<commit_message>
create template .csvs for better data handling
</commit_message>
<xml_diff>
--- a/inputs/template_event.xlsx
+++ b/inputs/template_event.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bellwethereducation-my.sharepoint.com/personal/marisa_mission_bellwether_org/Documents/Documents/MNM templates and references/data science stuff/R Projects/bw-event-planner/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_DEE5E034C55E9CE1530883576A803D3F4510069C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1573A8C7-C572-4B07-853A-11B2CEA38DED}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="11_DEE5E034C55E9CE1530883576A803D3F4510069C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3256D069-9C23-4EC4-949E-CC4692833DE5}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-684" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -96,9 +96,6 @@
   </si>
   <si>
     <t>Event Name:</t>
-  </si>
-  <si>
-    <t>{{Include answer from user input}}</t>
   </si>
   <si>
     <t>Event Dates:</t>
@@ -262,12 +259,15 @@
   <si>
     <t>A budget tracker within your PM doc is helpful</t>
   </si>
+  <si>
+    <t>{{answer from user input}}</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -297,6 +297,11 @@
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
@@ -707,7 +712,9 @@
   </sheetPr>
   <dimension ref="A1:Z1020"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -723,7 +730,7 @@
         <v>24</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>25</v>
+        <v>79</v>
       </c>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
@@ -752,10 +759,10 @@
     </row>
     <row r="2" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>25</v>
+        <v>79</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -784,10 +791,10 @@
     </row>
     <row r="3" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>25</v>
+        <v>79</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -816,10 +823,10 @@
     </row>
     <row r="4" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>25</v>
+        <v>79</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -848,10 +855,10 @@
     </row>
     <row r="5" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>25</v>
+        <v>79</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
@@ -880,10 +887,10 @@
     </row>
     <row r="6" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>25</v>
+        <v>79</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -941,22 +948,22 @@
     <row r="8" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5"/>
       <c r="B8" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="D8" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="E8" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="F8" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="G8" s="5" t="s">
         <v>35</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>36</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -980,7 +987,7 @@
     </row>
     <row r="9" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -1011,15 +1018,15 @@
     <row r="10" spans="1:26" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5"/>
       <c r="B10" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G10" s="7"/>
       <c r="H10" s="8"/>
@@ -1045,11 +1052,11 @@
     <row r="11" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5"/>
       <c r="B11" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="9"/>
@@ -1076,7 +1083,7 @@
     </row>
     <row r="12" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -1107,11 +1114,11 @@
     <row r="13" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5"/>
       <c r="B13" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="9"/>
@@ -1139,11 +1146,11 @@
     <row r="14" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5"/>
       <c r="B14" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="9"/>
@@ -1170,17 +1177,17 @@
     </row>
     <row r="15" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
       <c r="D15" s="10"/>
       <c r="E15" s="7"/>
       <c r="F15" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H15" s="8"/>
       <c r="I15" s="8"/>
@@ -1205,16 +1212,16 @@
     <row r="16" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5"/>
       <c r="B16" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E16" s="7"/>
       <c r="F16" s="9"/>
       <c r="G16" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H16" s="8"/>
       <c r="I16" s="8"/>
@@ -1239,11 +1246,11 @@
     <row r="17" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5"/>
       <c r="B17" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E17" s="7"/>
       <c r="F17" s="9"/>
@@ -1271,11 +1278,11 @@
     <row r="18" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5"/>
       <c r="B18" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="9"/>
@@ -1303,11 +1310,11 @@
     <row r="19" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5"/>
       <c r="B19" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C19" s="7"/>
       <c r="D19" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="9"/>
@@ -1334,7 +1341,7 @@
     </row>
     <row r="20" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
@@ -1365,16 +1372,16 @@
     <row r="21" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5"/>
       <c r="B21" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E21" s="7"/>
       <c r="F21" s="9"/>
       <c r="G21" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H21" s="8"/>
       <c r="I21" s="8"/>
@@ -1399,15 +1406,15 @@
     <row r="22" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="5"/>
       <c r="B22" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E22" s="7"/>
       <c r="F22" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G22" s="7"/>
       <c r="H22" s="8"/>
@@ -1432,7 +1439,7 @@
     </row>
     <row r="23" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
@@ -1463,16 +1470,16 @@
     <row r="24" spans="1:26" ht="57" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="5"/>
       <c r="B24" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C24" s="7"/>
       <c r="D24" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E24" s="7"/>
       <c r="F24" s="9"/>
       <c r="G24" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H24" s="8"/>
       <c r="I24" s="8"/>
@@ -1497,11 +1504,11 @@
     <row r="25" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="5"/>
       <c r="B25" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C25" s="7"/>
       <c r="D25" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E25" s="7"/>
       <c r="F25" s="9"/>
@@ -1529,11 +1536,11 @@
     <row r="26" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="5"/>
       <c r="B26" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C26" s="7"/>
       <c r="D26" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E26" s="7"/>
       <c r="F26" s="9"/>
@@ -1560,17 +1567,17 @@
     </row>
     <row r="27" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
       <c r="D27" s="10"/>
       <c r="E27" s="7"/>
       <c r="F27" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H27" s="8"/>
       <c r="I27" s="8"/>
@@ -1595,11 +1602,11 @@
     <row r="28" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="5"/>
       <c r="B28" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C28" s="7"/>
       <c r="D28" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E28" s="7"/>
       <c r="F28" s="9"/>
@@ -1627,11 +1634,11 @@
     <row r="29" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="5"/>
       <c r="B29" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C29" s="7"/>
       <c r="D29" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E29" s="7"/>
       <c r="F29" s="9"/>
@@ -1659,15 +1666,15 @@
     <row r="30" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="5"/>
       <c r="B30" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C30" s="7"/>
       <c r="D30" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E30" s="7"/>
       <c r="F30" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G30" s="7"/>
       <c r="H30" s="8"/>
@@ -1693,15 +1700,15 @@
     <row r="31" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="5"/>
       <c r="B31" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C31" s="7"/>
       <c r="D31" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E31" s="7"/>
       <c r="F31" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G31" s="7"/>
       <c r="H31" s="8"/>
@@ -1727,16 +1734,16 @@
     <row r="32" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="5"/>
       <c r="B32" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C32" s="7"/>
       <c r="D32" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E32" s="7"/>
       <c r="F32" s="9"/>
       <c r="G32" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H32" s="8"/>
       <c r="I32" s="8"/>
@@ -1761,11 +1768,11 @@
     <row r="33" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="5"/>
       <c r="B33" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C33" s="7"/>
       <c r="D33" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E33" s="7"/>
       <c r="F33" s="9"/>
@@ -1793,11 +1800,11 @@
     <row r="34" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="5"/>
       <c r="B34" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C34" s="7"/>
       <c r="D34" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E34" s="7"/>
       <c r="F34" s="9"/>
@@ -1825,11 +1832,11 @@
     <row r="35" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="5"/>
       <c r="B35" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C35" s="7"/>
       <c r="D35" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E35" s="7"/>
       <c r="F35" s="9"/>
@@ -1856,7 +1863,7 @@
     </row>
     <row r="36" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
@@ -1887,11 +1894,11 @@
     <row r="37" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="5"/>
       <c r="B37" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C37" s="7"/>
       <c r="D37" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E37" s="7"/>
       <c r="F37" s="9"/>
@@ -1919,11 +1926,11 @@
     <row r="38" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="5"/>
       <c r="B38" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C38" s="7"/>
       <c r="D38" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E38" s="7"/>
       <c r="F38" s="9"/>
@@ -1951,11 +1958,11 @@
     <row r="39" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="5"/>
       <c r="B39" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C39" s="7"/>
       <c r="D39" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E39" s="7"/>
       <c r="F39" s="9"/>
@@ -1982,7 +1989,7 @@
     </row>
     <row r="40" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B40" s="7"/>
       <c r="C40" s="7"/>
@@ -2013,11 +2020,11 @@
     <row r="41" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="5"/>
       <c r="B41" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C41" s="7"/>
       <c r="D41" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E41" s="7"/>
       <c r="F41" s="9"/>
@@ -2044,7 +2051,7 @@
     </row>
     <row r="42" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
@@ -2075,11 +2082,11 @@
     <row r="43" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="5"/>
       <c r="B43" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C43" s="7"/>
       <c r="D43" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E43" s="7"/>
       <c r="F43" s="9"/>
@@ -2107,16 +2114,16 @@
     <row r="44" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="5"/>
       <c r="B44" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C44" s="7"/>
       <c r="D44" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E44" s="7"/>
       <c r="F44" s="9"/>
       <c r="G44" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H44" s="8"/>
       <c r="I44" s="8"/>
@@ -29467,6 +29474,7 @@
       <c r="Z1020" s="8"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C10:C11 C13:C14 C16:C19 C21:C22 C24:C26 C28:C35 C37:C39 C41 C43:C44" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Alex,Amy,Biko,Nick"</formula1>

</xml_diff>